<commit_message>
Updated ID - Authentication Query
</commit_message>
<xml_diff>
--- a/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
+++ b/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pws.mindtree.com/projects/NP-087/Docs/Requirements/Logs-Trackers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100002_{BF016204-7A4D-4CAE-A182-4F668DD8B7D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17403CED-66B9-4345-BF9E-87F58C8389C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3405" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="967">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -11262,6 +11262,66 @@
         <family val="1"/>
       </rPr>
       <t>TBD with Anadi for clarity on the reason</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Parameters in e-KYC api:
+1. Status:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> As per Aadhaar Api status means  high level status of the API call. It can have values “0” or “-1”. If the status is “0”, it means that the encrypted data contained within the “Resp” element is valid. If it contains “-1”, it means the data should not be decrypted and used.
+What is the need of this parameter? In which scenario this is getting used?
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>KO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: As per Aadhaar Api  this attribute contains either value “KUA”, “ASA” or “” based on whose key was used to encrypt. If there were any errors (when “status” is “-1”), this attribute will have blank value
+Why should an ASA be allowed to encrpt/decrypt the request/response?
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wadh: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>What is the significnce of this element in e-KYC and other authentication APIs of Aadhaar?
+4. Authentication request(rad) and response (rar) within eKYC  are encoded and not encrpted in Aadhaar API. What is the reason behind this?
+5. Why there is no element in eKYC API for the requestor's digital signature? 
+6. What is the significance of the "txn" attribute in the API in case of e-KYC or BFD cases?</t>
     </r>
   </si>
 </sst>
@@ -21203,8 +21263,8 @@
   <dimension ref="A1:M212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
+      <pane ySplit="2" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G208" sqref="G208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -28789,14 +28849,28 @@
       </c>
       <c r="M207" s="12"/>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A208" s="66"/>
-      <c r="B208" s="9"/>
-      <c r="C208" s="9"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="11"/>
-      <c r="F208" s="11"/>
-      <c r="G208" s="12"/>
+    <row r="208" spans="1:13" ht="399" x14ac:dyDescent="0.25">
+      <c r="A208" s="66">
+        <v>206</v>
+      </c>
+      <c r="B208" s="10">
+        <v>43412</v>
+      </c>
+      <c r="C208" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D208" s="62" t="s">
+        <v>918</v>
+      </c>
+      <c r="E208" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F208" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="G208" s="47" t="s">
+        <v>966</v>
+      </c>
       <c r="H208" s="9"/>
       <c r="I208" s="13"/>
       <c r="J208" s="12"/>
@@ -29096,29 +29170,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29329,27 +29386,35 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29374,9 +29439,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Queries for ID-Authentication module
</commit_message>
<xml_diff>
--- a/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
+++ b/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17403CED-66B9-4345-BF9E-87F58C8389C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5C85445-6E0A-48BB-ADB1-DB33D00E5AC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3410" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="970">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -11323,6 +11323,17 @@
 5. Why there is no element in eKYC API for the requestor's digital signature? 
 6. What is the significance of the "txn" attribute in the API in case of e-KYC or BFD cases?</t>
     </r>
+  </si>
+  <si>
+    <t>Annexure D - Functional Requirement Specification dtd 15062018 [F]</t>
+  </si>
+  <si>
+    <t>For Fingerprint Authentication implementation in  Morrocco, which of the two approaches is finalised
+a)the system should be able to send the request to CNIE and receive the authentication response
+b)the system should be able to retrieve the CNIE number and the corresponding fingerprint minutae from CNIE fingerprint library hosted in RNP data centre</t>
+  </si>
+  <si>
+    <t>As per Aadhaar, the biometric modalities (Face/Finger/IRIS) should not exceed 2. Why is this restriction imposed?</t>
   </si>
 </sst>
 </file>
@@ -18387,7 +18398,7 @@
       <c r="M157" s="10"/>
       <c r="N157" s="12"/>
     </row>
-    <row r="158" spans="1:14" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="171" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <v>155</v>
       </c>
@@ -21263,8 +21274,8 @@
   <dimension ref="A1:M212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G208" sqref="G208"/>
+      <pane ySplit="2" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G209" sqref="G209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -28878,14 +28889,28 @@
       <c r="L208" s="9"/>
       <c r="M208" s="12"/>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A209" s="66"/>
-      <c r="B209" s="9"/>
-      <c r="C209" s="9"/>
-      <c r="D209" s="12"/>
-      <c r="E209" s="11"/>
-      <c r="F209" s="11"/>
-      <c r="G209" s="12"/>
+    <row r="209" spans="1:13" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="A209" s="66">
+        <v>207</v>
+      </c>
+      <c r="B209" s="10">
+        <v>43423</v>
+      </c>
+      <c r="C209" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D209" s="12" t="s">
+        <v>967</v>
+      </c>
+      <c r="E209" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F209" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="G209" s="12" t="s">
+        <v>968</v>
+      </c>
       <c r="H209" s="9"/>
       <c r="I209" s="13"/>
       <c r="J209" s="12"/>
@@ -28893,14 +28918,28 @@
       <c r="L209" s="9"/>
       <c r="M209" s="12"/>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A210" s="66"/>
-      <c r="B210" s="9"/>
-      <c r="C210" s="9"/>
-      <c r="D210" s="12"/>
-      <c r="E210" s="11"/>
-      <c r="F210" s="11"/>
-      <c r="G210" s="12"/>
+    <row r="210" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A210" s="66">
+        <v>208</v>
+      </c>
+      <c r="B210" s="10">
+        <v>43423</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D210" s="12" t="s">
+        <v>824</v>
+      </c>
+      <c r="E210" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F210" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="G210" s="12" t="s">
+        <v>969</v>
+      </c>
       <c r="H210" s="9"/>
       <c r="I210" s="13"/>
       <c r="J210" s="12"/>
@@ -29170,12 +29209,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29386,35 +29442,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29439,18 +29487,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated ID Authentication questions
</commit_message>
<xml_diff>
--- a/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
+++ b/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A5C85445-6E0A-48BB-ADB1-DB33D00E5AC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB2EE1E6-76F5-4952-A9B1-2E49467515E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="971">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -11334,6 +11334,30 @@
   </si>
   <si>
     <t>As per Aadhaar, the biometric modalities (Face/Finger/IRIS) should not exceed 2. Why is this restriction imposed?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Registered device Service in Biometric Authentication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. What is RD Service? How is it related to authentication of Biometric Devices? 
+2. What are dpId, rdsId, rdsVer, dc and mc as returned by RD Service? 
+3. what is the dih element which is supposed to be calculated by RD Service and sent as part of Auth Request?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -21275,7 +21299,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G209" sqref="G209"/>
+      <selection pane="bottomLeft" activeCell="G211" sqref="G211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -28947,14 +28971,28 @@
       <c r="L210" s="9"/>
       <c r="M210" s="12"/>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A211" s="66"/>
-      <c r="B211" s="9"/>
-      <c r="C211" s="9"/>
-      <c r="D211" s="12"/>
-      <c r="E211" s="11"/>
-      <c r="F211" s="11"/>
-      <c r="G211" s="12"/>
+    <row r="211" spans="1:13" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A211" s="66">
+        <v>209</v>
+      </c>
+      <c r="B211" s="10">
+        <v>43424</v>
+      </c>
+      <c r="C211" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D211" s="12" t="s">
+        <v>824</v>
+      </c>
+      <c r="E211" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F211" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="G211" s="12" t="s">
+        <v>970</v>
+      </c>
       <c r="H211" s="9"/>
       <c r="I211" s="13"/>
       <c r="J211" s="12"/>
@@ -29235,6 +29273,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -29441,15 +29488,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
@@ -29468,6 +29506,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1DD169-1613-4852-8D49-4C3CB1FDBF80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29484,12 +29530,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated a Query - IDA
</commit_message>
<xml_diff>
--- a/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
+++ b/requirements/MasterWeeklyQueryLog_MOSIP_18Sep18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB2EE1E6-76F5-4952-A9B1-2E49467515E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3EE51766-6716-4862-B46F-73373C615F9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3428" uniqueCount="974">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -11325,14 +11325,6 @@
     </r>
   </si>
   <si>
-    <t>Annexure D - Functional Requirement Specification dtd 15062018 [F]</t>
-  </si>
-  <si>
-    <t>For Fingerprint Authentication implementation in  Morrocco, which of the two approaches is finalised
-a)the system should be able to send the request to CNIE and receive the authentication response
-b)the system should be able to retrieve the CNIE number and the corresponding fingerprint minutae from CNIE fingerprint library hosted in RNP data centre</t>
-  </si>
-  <si>
     <t>As per Aadhaar, the biometric modalities (Face/Finger/IRIS) should not exceed 2. Why is this restriction imposed?</t>
   </si>
   <si>
@@ -11358,6 +11350,36 @@
 2. What are dpId, rdsId, rdsVer, dc and mc as returned by RD Service? 
 3. what is the dih element which is supposed to be calculated by RD Service and sent as part of Auth Request?</t>
     </r>
+  </si>
+  <si>
+    <t>Tracked in JIRA MOS-9748</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mail dated Nov 21 on </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Clarification Sent to GoM on CNIE, UIN, etc ..</t>
+    </r>
+  </si>
+  <si>
+    <t>Tracked in JIRA MOS-9749</t>
+  </si>
+  <si>
+    <t>Tracked in JIRA MOS-9750</t>
+  </si>
+  <si>
+    <t>1. What is Data Enrichment Services? What should these services do ? Does MOSIP have to develop these services?
+2. Please confirm that we have to retrieve only fingerprints and not any other biometric/demo data from CNIE?
+3. Please confirm the fingerprints will be pushed from CNIE to MOSIP. In that case when will this data be pushed?
+4. 'MOSIP will review &amp; support the entire process flow for CNIE integration as being developed under supervision of GoM for critical feedback &amp; suggestions'. What part of this feature will be under MVP and what will be considered later as a change request?</t>
   </si>
 </sst>
 </file>
@@ -21299,7 +21321,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G211" sqref="G211"/>
+      <selection pane="bottomLeft" activeCell="G209" sqref="G209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -28908,12 +28930,14 @@
       </c>
       <c r="H208" s="9"/>
       <c r="I208" s="13"/>
-      <c r="J208" s="12"/>
+      <c r="J208" s="12" t="s">
+        <v>969</v>
+      </c>
       <c r="K208" s="9"/>
       <c r="L208" s="9"/>
       <c r="M208" s="12"/>
     </row>
-    <row r="209" spans="1:13" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A209" s="66">
         <v>207</v>
       </c>
@@ -28924,7 +28948,7 @@
         <v>39</v>
       </c>
       <c r="D209" s="12" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
       <c r="E209" s="11" t="s">
         <v>35</v>
@@ -28933,7 +28957,7 @@
         <v>654</v>
       </c>
       <c r="G209" s="12" t="s">
-        <v>968</v>
+        <v>973</v>
       </c>
       <c r="H209" s="9"/>
       <c r="I209" s="13"/>
@@ -28962,11 +28986,13 @@
         <v>654</v>
       </c>
       <c r="G210" s="12" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="H210" s="9"/>
       <c r="I210" s="13"/>
-      <c r="J210" s="12"/>
+      <c r="J210" s="12" t="s">
+        <v>971</v>
+      </c>
       <c r="K210" s="9"/>
       <c r="L210" s="9"/>
       <c r="M210" s="12"/>
@@ -28991,17 +29017,21 @@
         <v>654</v>
       </c>
       <c r="G211" s="12" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="H211" s="9"/>
       <c r="I211" s="13"/>
-      <c r="J211" s="12"/>
+      <c r="J211" s="12" t="s">
+        <v>972</v>
+      </c>
       <c r="K211" s="9"/>
       <c r="L211" s="9"/>
       <c r="M211" s="12"/>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A212" s="66"/>
+      <c r="A212" s="66">
+        <v>210</v>
+      </c>
       <c r="B212" s="9"/>
       <c r="C212" s="9"/>
       <c r="D212" s="12"/>
@@ -29247,6 +29277,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -29270,15 +29309,6 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29489,6 +29519,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -29501,14 +29539,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>